<commit_message>
front controlleur + uptade sprint
</commit_message>
<xml_diff>
--- a/c-61/sprint0/Planification.xlsx
+++ b/c-61/sprint0/Planification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15148\Desktop\ProjetSynthese\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koral\eclipse-workspace\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5651A5A-3636-4BDF-8A5E-6775670D4A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72E8A4F-B54A-49E7-8504-3C4A9A4F8984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-5145" windowWidth="25440" windowHeight="15390" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
+    <workbookView xWindow="32115" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
   <si>
     <t>Numéro de tâche</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Titre du projet</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -345,7 +348,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -709,15 +712,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -728,15 +722,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -754,11 +739,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,96 +839,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,7 +881,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1176,115 +1179,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB36122-9B2D-4250-BEE7-2344E7EABB3F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="E1" s="52"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
-      <c r="B3" s="54" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="52"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
+      <c r="B3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="43" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="54" t="s">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="21">
         <f>Sprints!A17</f>
         <v>13</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="22">
         <f>Sprints!A25</f>
         <v>5</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="23">
         <f>Sprints!A36</f>
         <v>8</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="46">
         <f>SUM(B4:D4)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="54" t="s">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="24">
         <f>Sprints!H17/2</f>
         <v>28</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="25">
         <f>Sprints!H25/2</f>
         <v>19</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="26">
         <f>Sprints!H36/2</f>
         <v>20</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="47">
         <f>SUM(B5:D5)</f>
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="44">
         <f>SUM(Sprints!G3:G15)/Sprints!A17</f>
         <v>3.8076923076923075</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="44">
         <f>SUM(Sprints!G19:G23)/Sprints!A25</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="45">
         <f>SUM(Sprints!G27:G34)/Sprints!A36</f>
         <v>2.0000000000000004</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="44">
         <f>SUM(B6:D6)/3</f>
         <v>3.5692307692307694</v>
       </c>
@@ -1303,40 +1306,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0FA19E-15D0-43BC-BF02-687111E69EB6}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="13.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="2"/>
     <col min="10" max="10" width="46" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1367,416 +1370,420 @@
       <c r="J2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="23"/>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37">
-        <v>1</v>
-      </c>
-      <c r="B3" s="38" t="s">
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="29">
         <v>10</v>
       </c>
-      <c r="G3" s="47" cm="1">
+      <c r="G3" s="36" cm="1">
         <f t="array" ref="G3">SUM($F$3:$F$15)*(H3*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>7.9838709677419351</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="29">
         <v>10</v>
       </c>
-      <c r="I3" s="38">
-        <v>1</v>
-      </c>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="40">
+      <c r="I3" s="29">
+        <v>1</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="25" cm="1">
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19" cm="1">
         <f t="array" ref="G4">SUM($F$3:$F$15)*(H4*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>2</v>
       </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="41"/>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="40">
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="14">
-        <v>1</v>
-      </c>
-      <c r="G5" s="25" cm="1">
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" cm="1">
         <f t="array" ref="G5">SUM($F$3:$F$15)*(H5*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>4.790322580645161</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="11">
         <v>6</v>
       </c>
-      <c r="I5" s="14">
-        <v>1</v>
-      </c>
-      <c r="J5" s="41"/>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40">
+      <c r="I5" s="11">
+        <v>1</v>
+      </c>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25" cm="1">
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19" cm="1">
         <f t="array" ref="G6">SUM($F$3:$F$15)*(H6*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>2</v>
       </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="41"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="40">
+      <c r="I6" s="11">
+        <v>1</v>
+      </c>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="14">
-        <v>1</v>
-      </c>
-      <c r="G7" s="25" cm="1">
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="19" cm="1">
         <f t="array" ref="G7">SUM($F$3:$F$15)*(H7*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="11">
         <v>2</v>
       </c>
-      <c r="I7" s="14">
-        <v>1</v>
-      </c>
-      <c r="J7" s="41"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="40">
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <v>7.5</v>
       </c>
-      <c r="G8" s="25" cm="1">
+      <c r="G8" s="19" cm="1">
         <f t="array" ref="G8">SUM($F$3:$F$15)*(H8*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>6.387096774193548</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="11">
         <v>8</v>
       </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="41"/>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40">
+      <c r="I8" s="11">
+        <v>1</v>
+      </c>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <v>7.5</v>
       </c>
-      <c r="G9" s="25" cm="1">
+      <c r="G9" s="19" cm="1">
         <f t="array" ref="G9">SUM($F$3:$F$15)*(H9*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="11">
         <v>2</v>
       </c>
-      <c r="I9" s="14">
-        <v>1</v>
-      </c>
-      <c r="J9" s="41"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40">
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="25" cm="1">
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+      <c r="G10" s="19" cm="1">
         <f t="array" ref="G10">SUM($F$3:$F$15)*(H10*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <v>2</v>
       </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="41"/>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40">
+      <c r="I10" s="11">
+        <v>1</v>
+      </c>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
         <v>9</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>5</v>
       </c>
-      <c r="G11" s="25" cm="1">
+      <c r="G11" s="19" cm="1">
         <f t="array" ref="G11">SUM($F$3:$F$15)*(H11*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>4.790322580645161</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="11">
         <v>6</v>
       </c>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40">
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="25" cm="1">
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19" cm="1">
         <f t="array" ref="G12">SUM($F$3:$F$15)*(H12*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="11">
         <v>2</v>
       </c>
-      <c r="I12" s="14">
-        <v>1</v>
-      </c>
-      <c r="J12" s="41"/>
-      <c r="L12" s="24"/>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="40">
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <v>5</v>
       </c>
-      <c r="G13" s="25" cm="1">
+      <c r="G13" s="19" cm="1">
         <f t="array" ref="G13">SUM($F$3:$F$15)*(H13*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>3.193548387096774</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="11">
         <v>4</v>
       </c>
-      <c r="I13" s="14">
-        <v>1</v>
-      </c>
-      <c r="J13" s="41"/>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="40">
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <v>7.5</v>
       </c>
-      <c r="G14" s="25" cm="1">
+      <c r="G14" s="19" cm="1">
         <f t="array" ref="G14">SUM($F$3:$F$15)*(H14*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>7.9838709677419351</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="11">
         <v>10</v>
       </c>
-      <c r="I14" s="14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="41" t="s">
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="44">
+    <row r="15" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="26" cm="1">
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20" cm="1">
         <f t="array" ref="G15">SUM($F$3:$F$15)*(H15*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>4.790322580645161</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="12">
         <v>6</v>
       </c>
-      <c r="I15" s="15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="46" t="s">
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:13" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="5"/>
@@ -1785,13 +1792,13 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="47.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f>COUNT(A3:A15)</f>
         <v>13</v>
@@ -1800,8 +1807,8 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="53">
+      <c r="F17" s="40"/>
+      <c r="G17" s="42">
         <f>SUM(G3:G15)/A17</f>
         <v>3.8076923076923075</v>
       </c>
@@ -1814,179 +1821,179 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="37">
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="58"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
         <v>14</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="29">
         <v>7.5</v>
       </c>
-      <c r="G19" s="47" cm="1">
+      <c r="G19" s="36" cm="1">
         <f t="array" ref="G19">SUM($F$19:$F$23)*(H19*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>10.315789473684211</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="29">
         <v>16</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="29">
         <v>2</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
         <v>15</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="14">
-        <v>1</v>
-      </c>
-      <c r="G20" s="25" cm="1">
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="19" cm="1">
         <f t="array" ref="G20">SUM($F$19:$F$23)*(H20*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>1.2894736842105263</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="11">
         <v>2</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="11">
         <v>2</v>
       </c>
-      <c r="J20" s="41"/>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40">
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
         <v>16</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="14">
-        <v>1</v>
-      </c>
-      <c r="G21" s="25" cm="1">
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="19" cm="1">
         <f t="array" ref="G21">SUM($F$19:$F$23)*(H21*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>1.2894736842105263</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="11">
         <v>2</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="11">
         <v>2</v>
       </c>
-      <c r="J21" s="41"/>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="40">
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
         <v>17</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="11">
         <v>10</v>
       </c>
-      <c r="G22" s="25" cm="1">
+      <c r="G22" s="19" cm="1">
         <f t="array" ref="G22">SUM($F$19:$F$23)*(H22*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>6.4473684210526319</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="11">
         <v>10</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="11">
         <v>2</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="44">
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
         <v>18</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="12">
         <v>5</v>
       </c>
-      <c r="G23" s="26" cm="1">
+      <c r="G23" s="20" cm="1">
         <f t="array" ref="G23">SUM($F$19:$F$23)*(H23*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>5.1578947368421053</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="12">
         <v>8</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="12">
         <v>2</v>
       </c>
-      <c r="J23" s="46"/>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="5"/>
@@ -1995,19 +2002,19 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <f>COUNT(A19:A23)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53">
+      <c r="F25" s="41"/>
+      <c r="G25" s="42">
         <f>SUM(G19:G24)/A25</f>
         <v>4.9000000000000004</v>
       </c>
@@ -2016,264 +2023,264 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="37">
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
+    </row>
+    <row r="27" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="28">
         <v>19</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="29">
         <v>5</v>
       </c>
-      <c r="G27" s="38" cm="1">
+      <c r="G27" s="29" cm="1">
         <f t="array" ref="G27">SUM($F$27:$F$34)*(H27*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>4</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="29">
         <v>10</v>
       </c>
-      <c r="I27" s="38">
+      <c r="I27" s="29">
         <v>3</v>
       </c>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40">
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
         <v>20</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="11">
         <v>5</v>
       </c>
-      <c r="G28" s="14" cm="1">
+      <c r="G28" s="11" cm="1">
         <f t="array" ref="G28">SUM($F$27:$F$34)*(H28*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>2.4</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="11">
         <v>6</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="11">
         <v>3</v>
       </c>
-      <c r="J28" s="41"/>
-    </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40">
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
         <v>21</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="14">
-        <v>1</v>
-      </c>
-      <c r="G29" s="14" cm="1">
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+      <c r="G29" s="11" cm="1">
         <f t="array" ref="G29">SUM($F$27:$F$34)*(H29*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>2.4</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="11">
         <v>6</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="11">
         <v>3</v>
       </c>
-      <c r="J29" s="41"/>
-    </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40">
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
         <v>22</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="14">
-        <v>1</v>
-      </c>
-      <c r="G30" s="14" cm="1">
+      <c r="F30" s="11">
+        <v>1</v>
+      </c>
+      <c r="G30" s="11" cm="1">
         <f t="array" ref="G30">SUM($F$27:$F$34)*(H30*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>1.6</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="11">
         <v>4</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="11">
         <v>3</v>
       </c>
-      <c r="J30" s="41"/>
-    </row>
-    <row r="31" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="40">
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
         <v>23</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="14">
-        <v>1</v>
-      </c>
-      <c r="G31" s="14" cm="1">
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11" cm="1">
         <f t="array" ref="G31">SUM($F$27:$F$34)*(H31*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>0.8</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="11">
         <v>2</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="11">
         <v>3</v>
       </c>
-      <c r="J31" s="41"/>
-    </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="40">
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
         <v>24</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="14">
-        <v>1</v>
-      </c>
-      <c r="G32" s="14" cm="1">
+      <c r="F32" s="11">
+        <v>1</v>
+      </c>
+      <c r="G32" s="11" cm="1">
         <f t="array" ref="G32">SUM($F$27:$F$34)*(H32*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>2.4</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="11">
         <v>6</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="11">
         <v>3</v>
       </c>
-      <c r="J32" s="42"/>
-    </row>
-    <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="40">
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
         <v>25</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="14">
-        <v>1</v>
-      </c>
-      <c r="G33" s="14" cm="1">
+      <c r="F33" s="11">
+        <v>1</v>
+      </c>
+      <c r="G33" s="11" cm="1">
         <f t="array" ref="G33">SUM($F$27:$F$34)*(H33*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>0.8</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="11">
         <v>2</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="11">
         <v>3</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="44">
+    <row r="34" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="34">
         <v>26</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="15" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="15">
-        <v>1</v>
-      </c>
-      <c r="G34" s="15" cm="1">
+      <c r="F34" s="12">
+        <v>1</v>
+      </c>
+      <c r="G34" s="12" cm="1">
         <f t="array" ref="G34">SUM($F$27:$F$34)*(H34*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>1.6</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="12">
         <v>4</v>
       </c>
-      <c r="I34" s="15">
+      <c r="I34" s="12">
         <v>3</v>
       </c>
-      <c r="J34" s="45"/>
-    </row>
-    <row r="35" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
+      <c r="J34" s="60"/>
+    </row>
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="5"/>
@@ -2282,19 +2289,19 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="48">
+    <row r="36" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37">
         <f>COUNT(A27:A34)</f>
         <v>8</v>
       </c>
       <c r="B36" s="9"/>
-      <c r="C36" s="49"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -2304,9 +2311,9 @@
         <v>40</v>
       </c>
       <c r="I36" s="9"/>
-      <c r="J36" s="50"/>
-    </row>
-    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="39"/>
+    </row>
+    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
@@ -2316,7 +2323,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
@@ -2326,7 +2333,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
@@ -2336,8 +2343,8 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C45" s="36"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
user dao + dao config aggisant en tant que superclasse
</commit_message>
<xml_diff>
--- a/c-61/sprint0/Planification.xlsx
+++ b/c-61/sprint0/Planification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15148\Desktop\ProjetSynthese\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koral\Documents\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5651A5A-3636-4BDF-8A5E-6775670D4A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A15D1F-A767-471A-B76E-2285FC887F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-5145" windowWidth="25440" windowHeight="15390" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
+    <workbookView xWindow="32115" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
   <si>
     <t>Numéro de tâche</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>Titre du projet</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>mysql done</t>
   </si>
 </sst>
 </file>
@@ -345,7 +351,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -709,15 +715,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -728,15 +725,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -754,11 +742,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,96 +842,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,7 +884,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1176,115 +1182,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB36122-9B2D-4250-BEE7-2344E7EABB3F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="E1" s="52"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
-      <c r="B3" s="54" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="52"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
+      <c r="B3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="43" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="54" t="s">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="21">
         <f>Sprints!A17</f>
         <v>13</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="22">
         <f>Sprints!A25</f>
         <v>5</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="23">
         <f>Sprints!A36</f>
         <v>8</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="46">
         <f>SUM(B4:D4)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="54" t="s">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="24">
         <f>Sprints!H17/2</f>
         <v>28</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="25">
         <f>Sprints!H25/2</f>
         <v>19</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="26">
         <f>Sprints!H36/2</f>
         <v>20</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="47">
         <f>SUM(B5:D5)</f>
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="44">
         <f>SUM(Sprints!G3:G15)/Sprints!A17</f>
         <v>3.8076923076923075</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="44">
         <f>SUM(Sprints!G19:G23)/Sprints!A25</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="45">
         <f>SUM(Sprints!G27:G34)/Sprints!A36</f>
         <v>2.0000000000000004</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="44">
         <f>SUM(B6:D6)/3</f>
         <v>3.5692307692307694</v>
       </c>
@@ -1303,40 +1309,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0FA19E-15D0-43BC-BF02-687111E69EB6}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="13.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="2"/>
     <col min="10" max="10" width="46" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1367,416 +1373,422 @@
       <c r="J2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="23"/>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37">
-        <v>1</v>
-      </c>
-      <c r="B3" s="38" t="s">
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="29">
         <v>10</v>
       </c>
-      <c r="G3" s="47" cm="1">
+      <c r="G3" s="36" cm="1">
         <f t="array" ref="G3">SUM($F$3:$F$15)*(H3*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>7.9838709677419351</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="29">
         <v>10</v>
       </c>
-      <c r="I3" s="38">
-        <v>1</v>
-      </c>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="40">
+      <c r="I3" s="29">
+        <v>1</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="25" cm="1">
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19" cm="1">
         <f t="array" ref="G4">SUM($F$3:$F$15)*(H4*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>2</v>
       </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="41"/>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="40">
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="14">
-        <v>1</v>
-      </c>
-      <c r="G5" s="25" cm="1">
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" cm="1">
         <f t="array" ref="G5">SUM($F$3:$F$15)*(H5*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>4.790322580645161</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="11">
         <v>6</v>
       </c>
-      <c r="I5" s="14">
-        <v>1</v>
-      </c>
-      <c r="J5" s="41"/>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40">
+      <c r="I5" s="11">
+        <v>1</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25" cm="1">
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19" cm="1">
         <f t="array" ref="G6">SUM($F$3:$F$15)*(H6*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>2</v>
       </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="41"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="40">
+      <c r="I6" s="11">
+        <v>1</v>
+      </c>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="14">
-        <v>1</v>
-      </c>
-      <c r="G7" s="25" cm="1">
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="19" cm="1">
         <f t="array" ref="G7">SUM($F$3:$F$15)*(H7*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="11">
         <v>2</v>
       </c>
-      <c r="I7" s="14">
-        <v>1</v>
-      </c>
-      <c r="J7" s="41"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="40">
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <v>7.5</v>
       </c>
-      <c r="G8" s="25" cm="1">
+      <c r="G8" s="19" cm="1">
         <f t="array" ref="G8">SUM($F$3:$F$15)*(H8*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>6.387096774193548</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="11">
         <v>8</v>
       </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="41"/>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40">
+      <c r="I8" s="11">
+        <v>1</v>
+      </c>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <v>7.5</v>
       </c>
-      <c r="G9" s="25" cm="1">
+      <c r="G9" s="19" cm="1">
         <f t="array" ref="G9">SUM($F$3:$F$15)*(H9*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="11">
         <v>2</v>
       </c>
-      <c r="I9" s="14">
-        <v>1</v>
-      </c>
-      <c r="J9" s="41"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40">
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="25" cm="1">
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+      <c r="G10" s="19" cm="1">
         <f t="array" ref="G10">SUM($F$3:$F$15)*(H10*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <v>2</v>
       </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="41"/>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40">
+      <c r="I10" s="11">
+        <v>1</v>
+      </c>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
         <v>9</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>5</v>
       </c>
-      <c r="G11" s="25" cm="1">
+      <c r="G11" s="19" cm="1">
         <f t="array" ref="G11">SUM($F$3:$F$15)*(H11*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>4.790322580645161</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="11">
         <v>6</v>
       </c>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40">
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="25" cm="1">
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19" cm="1">
         <f t="array" ref="G12">SUM($F$3:$F$15)*(H12*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>1.596774193548387</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="11">
         <v>2</v>
       </c>
-      <c r="I12" s="14">
-        <v>1</v>
-      </c>
-      <c r="J12" s="41"/>
-      <c r="L12" s="24"/>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="40">
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <v>5</v>
       </c>
-      <c r="G13" s="25" cm="1">
+      <c r="G13" s="19" cm="1">
         <f t="array" ref="G13">SUM($F$3:$F$15)*(H13*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>3.193548387096774</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="11">
         <v>4</v>
       </c>
-      <c r="I13" s="14">
-        <v>1</v>
-      </c>
-      <c r="J13" s="41"/>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="40">
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <v>7.5</v>
       </c>
-      <c r="G14" s="25" cm="1">
+      <c r="G14" s="19" cm="1">
         <f t="array" ref="G14">SUM($F$3:$F$15)*(H14*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>7.9838709677419351</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="11">
         <v>10</v>
       </c>
-      <c r="I14" s="14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="41" t="s">
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="44">
+    <row r="15" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="26" cm="1">
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20" cm="1">
         <f t="array" ref="G15">SUM($F$3:$F$15)*(H15*60*2)/SUM($H$3:$H$15*2*60)</f>
         <v>4.790322580645161</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="12">
         <v>6</v>
       </c>
-      <c r="I15" s="15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="46" t="s">
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:13" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="5"/>
@@ -1785,13 +1797,13 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="47.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f>COUNT(A3:A15)</f>
         <v>13</v>
@@ -1800,8 +1812,8 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="53">
+      <c r="F17" s="40"/>
+      <c r="G17" s="42">
         <f>SUM(G3:G15)/A17</f>
         <v>3.8076923076923075</v>
       </c>
@@ -1814,179 +1826,179 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-    </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="37">
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="58"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
         <v>14</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="29">
         <v>7.5</v>
       </c>
-      <c r="G19" s="47" cm="1">
+      <c r="G19" s="36" cm="1">
         <f t="array" ref="G19">SUM($F$19:$F$23)*(H19*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>10.315789473684211</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="29">
         <v>16</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="29">
         <v>2</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
         <v>15</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="14">
-        <v>1</v>
-      </c>
-      <c r="G20" s="25" cm="1">
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="19" cm="1">
         <f t="array" ref="G20">SUM($F$19:$F$23)*(H20*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>1.2894736842105263</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="11">
         <v>2</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="11">
         <v>2</v>
       </c>
-      <c r="J20" s="41"/>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40">
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
         <v>16</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="14">
-        <v>1</v>
-      </c>
-      <c r="G21" s="25" cm="1">
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="19" cm="1">
         <f t="array" ref="G21">SUM($F$19:$F$23)*(H21*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>1.2894736842105263</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="11">
         <v>2</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="11">
         <v>2</v>
       </c>
-      <c r="J21" s="41"/>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="40">
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
         <v>17</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="11">
         <v>10</v>
       </c>
-      <c r="G22" s="25" cm="1">
+      <c r="G22" s="19" cm="1">
         <f t="array" ref="G22">SUM($F$19:$F$23)*(H22*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>6.4473684210526319</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="11">
         <v>10</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="11">
         <v>2</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="44">
+    <row r="23" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
         <v>18</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="12">
         <v>5</v>
       </c>
-      <c r="G23" s="26" cm="1">
+      <c r="G23" s="20" cm="1">
         <f t="array" ref="G23">SUM($F$19:$F$23)*(H23*60*2)/SUM($H$19:$H$23*2*60)</f>
         <v>5.1578947368421053</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="12">
         <v>8</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="12">
         <v>2</v>
       </c>
-      <c r="J23" s="46"/>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="5"/>
@@ -1995,19 +2007,19 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <f>COUNT(A19:A23)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53">
+      <c r="F25" s="41"/>
+      <c r="G25" s="42">
         <f>SUM(G19:G24)/A25</f>
         <v>4.9000000000000004</v>
       </c>
@@ -2016,264 +2028,264 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="37">
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
+    </row>
+    <row r="27" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="28">
         <v>19</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="29">
         <v>5</v>
       </c>
-      <c r="G27" s="38" cm="1">
+      <c r="G27" s="29" cm="1">
         <f t="array" ref="G27">SUM($F$27:$F$34)*(H27*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>4</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="29">
         <v>10</v>
       </c>
-      <c r="I27" s="38">
+      <c r="I27" s="29">
         <v>3</v>
       </c>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40">
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
         <v>20</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="11">
         <v>5</v>
       </c>
-      <c r="G28" s="14" cm="1">
+      <c r="G28" s="11" cm="1">
         <f t="array" ref="G28">SUM($F$27:$F$34)*(H28*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>2.4</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="11">
         <v>6</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="11">
         <v>3</v>
       </c>
-      <c r="J28" s="41"/>
-    </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40">
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
         <v>21</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="14">
-        <v>1</v>
-      </c>
-      <c r="G29" s="14" cm="1">
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+      <c r="G29" s="11" cm="1">
         <f t="array" ref="G29">SUM($F$27:$F$34)*(H29*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>2.4</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="11">
         <v>6</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="11">
         <v>3</v>
       </c>
-      <c r="J29" s="41"/>
-    </row>
-    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40">
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
         <v>22</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="14">
-        <v>1</v>
-      </c>
-      <c r="G30" s="14" cm="1">
+      <c r="F30" s="11">
+        <v>1</v>
+      </c>
+      <c r="G30" s="11" cm="1">
         <f t="array" ref="G30">SUM($F$27:$F$34)*(H30*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>1.6</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="11">
         <v>4</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="11">
         <v>3</v>
       </c>
-      <c r="J30" s="41"/>
-    </row>
-    <row r="31" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="40">
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
         <v>23</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="14">
-        <v>1</v>
-      </c>
-      <c r="G31" s="14" cm="1">
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11" cm="1">
         <f t="array" ref="G31">SUM($F$27:$F$34)*(H31*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>0.8</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="11">
         <v>2</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="11">
         <v>3</v>
       </c>
-      <c r="J31" s="41"/>
-    </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="40">
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
         <v>24</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="14">
-        <v>1</v>
-      </c>
-      <c r="G32" s="14" cm="1">
+      <c r="F32" s="11">
+        <v>1</v>
+      </c>
+      <c r="G32" s="11" cm="1">
         <f t="array" ref="G32">SUM($F$27:$F$34)*(H32*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>2.4</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="11">
         <v>6</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="11">
         <v>3</v>
       </c>
-      <c r="J32" s="42"/>
-    </row>
-    <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="40">
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
         <v>25</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="14">
-        <v>1</v>
-      </c>
-      <c r="G33" s="14" cm="1">
+      <c r="F33" s="11">
+        <v>1</v>
+      </c>
+      <c r="G33" s="11" cm="1">
         <f t="array" ref="G33">SUM($F$27:$F$34)*(H33*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>0.8</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="11">
         <v>2</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="11">
         <v>3</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="44">
+    <row r="34" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="34">
         <v>26</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="15" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="15">
-        <v>1</v>
-      </c>
-      <c r="G34" s="15" cm="1">
+      <c r="F34" s="12">
+        <v>1</v>
+      </c>
+      <c r="G34" s="12" cm="1">
         <f t="array" ref="G34">SUM($F$27:$F$34)*(H34*60*2)/SUM($H$27:$H$34*2*60)</f>
         <v>1.6</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="12">
         <v>4</v>
       </c>
-      <c r="I34" s="15">
+      <c r="I34" s="12">
         <v>3</v>
       </c>
-      <c r="J34" s="45"/>
-    </row>
-    <row r="35" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
+      <c r="J34" s="60"/>
+    </row>
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="5"/>
@@ -2282,19 +2294,19 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="48">
+    <row r="36" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37">
         <f>COUNT(A27:A34)</f>
         <v>8</v>
       </c>
       <c r="B36" s="9"/>
-      <c r="C36" s="49"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -2304,9 +2316,9 @@
         <v>40</v>
       </c>
       <c r="I36" s="9"/>
-      <c r="J36" s="50"/>
-    </row>
-    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="39"/>
+    </row>
+    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
@@ -2316,7 +2328,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
@@ -2326,7 +2338,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
@@ -2336,8 +2348,8 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C45" s="36"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
dernier version sans merge conflict
</commit_message>
<xml_diff>
--- a/c-61/sprint0/Planification.xlsx
+++ b/c-61/sprint0/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koral\eclipse-workspace\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72E8A4F-B54A-49E7-8504-3C4A9A4F8984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37E009A-328C-4A62-845C-F2454DCBFBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32115" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="3" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Numéro de tâche</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>mysql done</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1310,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1470,9 @@
       <c r="I5" s="11">
         <v>1</v>
       </c>
-      <c r="J5" s="32"/>
+      <c r="J5" s="32" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
@@ -1498,7 +1503,9 @@
       <c r="I6" s="11">
         <v>1</v>
       </c>
-      <c r="J6" s="32"/>
+      <c r="J6" s="32" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31">

</xml_diff>

<commit_message>
Add pom.properties to gitignore
</commit_message>
<xml_diff>
--- a/c-61/sprint0/Planification.xlsx
+++ b/c-61/sprint0/Planification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koral\Documents\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koral\eclipse-workspace\c-61-FrenetteKorallia-LemireWilliam\c-61\sprint0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A15D1F-A767-471A-B76E-2285FC887F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37E009A-328C-4A62-845C-F2454DCBFBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32115" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F453119D-F637-402F-92FD-C8ABCD52E234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="3" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Numéro de tâche</t>
   </si>
@@ -1310,7 +1310,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1503,9 @@
       <c r="I6" s="11">
         <v>1</v>
       </c>
-      <c r="J6" s="32"/>
+      <c r="J6" s="32" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31">

</xml_diff>